<commit_message>
Memory_Expansion_Daughter_Board: Updated PCB Design Checklist, still needing a lot of topics to cover #6
</commit_message>
<xml_diff>
--- a/Memory_Expansion_Daughter_Board/PCB Design Checklist.xlsx
+++ b/Memory_Expansion_Daughter_Board/PCB Design Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanaz\OneDrive\Área de Trabalho\SpaceLab\FloripaSat-2\Hardware Development\daughter_boards_obdh2\Memory_Expansion_Daughter_Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DE2AA5-3A10-4752-A948-5B7E5262EE61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4260F96-D298-4F71-9F4B-8799E7A9D1A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11670" yWindow="345" windowWidth="9165" windowHeight="7875" xr2:uid="{5735AEBB-7E66-4CF4-B607-EA3656031333}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5735AEBB-7E66-4CF4-B607-EA3656031333}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="171">
   <si>
     <t>1.</t>
   </si>
@@ -482,9 +482,6 @@
     <t>?</t>
   </si>
   <si>
-    <t>Needed?</t>
-  </si>
-  <si>
     <t>Using GPIO 4</t>
   </si>
   <si>
@@ -503,9 +500,6 @@
     <t>Reviewer and Support</t>
   </si>
   <si>
-    <t>OBDH 2.0 responsability</t>
-  </si>
-  <si>
     <t>Kleber Reis Gouveia Júnior</t>
   </si>
   <si>
@@ -518,13 +512,40 @@
     <t>Used lower values of capacitance due to project aplication.</t>
   </si>
   <si>
-    <t>What is uC programming???</t>
-  </si>
-  <si>
-    <t>Filters necessary???</t>
-  </si>
-  <si>
-    <t>FSI connector has 1.07 mm diameter alligment pin (AD version)</t>
+    <t>Added to "POWER TEST" pin connector</t>
+  </si>
+  <si>
+    <t>Not needed?</t>
+  </si>
+  <si>
+    <t>Same default thickness of OBDH 2.0</t>
+  </si>
+  <si>
+    <t>Only 2 layers.</t>
+  </si>
+  <si>
+    <t>Power width of 0.508mm and all other tracks with 0.254mm.</t>
+  </si>
+  <si>
+    <t>No polarity components on project.</t>
+  </si>
+  <si>
+    <t>Daughter Board PCB holes are standard for any aplication.</t>
+  </si>
+  <si>
+    <t>FSI connector has 1.07 mm diameter alligment pin (AD version).</t>
+  </si>
+  <si>
+    <t>OBDH 2.0 responsability.</t>
+  </si>
+  <si>
+    <t>Initial placement</t>
+  </si>
+  <si>
+    <t>4.4</t>
+  </si>
+  <si>
+    <t>4.5</t>
   </si>
 </sst>
 </file>
@@ -1085,10 +1106,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F77"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1101,7 +1122,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -1129,13 +1150,13 @@
         <v>68</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
@@ -1144,7 +1165,7 @@
       </c>
       <c r="E4" s="9">
         <f ca="1">NOW()</f>
-        <v>43883.460688425926</v>
+        <v>43886.891437615741</v>
       </c>
       <c r="F4" s="7"/>
     </row>
@@ -1185,11 +1206,13 @@
       <c r="B7" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="7" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1219,7 +1242,7 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1232,7 +1255,9 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="7"/>
+      <c r="F10" s="7" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
@@ -1244,7 +1269,9 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="7"/>
+      <c r="F11" s="7" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
@@ -1297,11 +1324,9 @@
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="2" t="s">
-        <v>134</v>
-      </c>
+      <c r="E15" s="2"/>
       <c r="F15" s="7" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1311,13 +1336,11 @@
       <c r="B16" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>134</v>
-      </c>
+      <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1333,7 +1356,7 @@
         <v>134</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1349,7 +1372,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1379,7 +1402,7 @@
         <v>134</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1403,7 +1426,9 @@
       <c r="B22" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="7"/>
@@ -1415,7 +1440,9 @@
       <c r="B23" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C23" s="2"/>
+      <c r="C23" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="7"/>
@@ -1457,7 +1484,9 @@
       <c r="B26" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="C26" s="2"/>
+      <c r="C26" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="7"/>
@@ -1475,7 +1504,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="7" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1500,11 +1529,13 @@
         <v>99</v>
       </c>
       <c r="C29" s="2"/>
-      <c r="D29" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="7"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
@@ -1525,10 +1556,14 @@
       <c r="B31" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="C31" s="2"/>
+      <c r="C31" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
-      <c r="F31" s="7"/>
+      <c r="F31" s="7" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
@@ -1549,10 +1584,14 @@
       <c r="B33" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C33" s="2"/>
+      <c r="C33" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
-      <c r="F33" s="7"/>
+      <c r="F33" s="7" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
@@ -1561,7 +1600,9 @@
       <c r="B34" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C34" s="2"/>
+      <c r="C34" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="7"/>
@@ -1573,7 +1614,9 @@
       <c r="B35" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C35" s="2"/>
+      <c r="C35" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="7"/>
@@ -1587,7 +1630,9 @@
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
+      <c r="E36" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="F36" s="7"/>
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1597,10 +1642,14 @@
       <c r="B37" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="C37" s="2"/>
+      <c r="C37" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
-      <c r="F37" s="7"/>
+      <c r="F37" s="7" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
@@ -1612,7 +1661,9 @@
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
-      <c r="F38" s="7"/>
+      <c r="F38" s="7" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
@@ -1621,10 +1672,14 @@
       <c r="B39" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="C39" s="2"/>
+      <c r="C39" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
-      <c r="F39" s="7"/>
+      <c r="F39" s="7" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
@@ -1635,7 +1690,9 @@
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
+      <c r="E40" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="F40" s="7"/>
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1647,7 +1704,9 @@
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
+      <c r="E41" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="F41" s="7"/>
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1657,7 +1716,9 @@
       <c r="B42" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="C42" s="2"/>
+      <c r="C42" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="7"/>
@@ -1681,7 +1742,9 @@
       <c r="B44" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="C44" s="2"/>
+      <c r="C44" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="7"/>
@@ -1707,8 +1770,12 @@
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="7"/>
+      <c r="E46" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
@@ -1720,7 +1787,9 @@
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
-      <c r="F47" s="7"/>
+      <c r="F47" s="7" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
@@ -1732,7 +1801,9 @@
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
-      <c r="F48" s="7"/>
+      <c r="F48" s="7" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
@@ -1744,7 +1815,9 @@
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
-      <c r="F49" s="7"/>
+      <c r="F49" s="7" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
@@ -1753,7 +1826,9 @@
       <c r="B50" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="C50" s="2"/>
+      <c r="C50" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="F50" s="7"/>
@@ -1765,7 +1840,9 @@
       <c r="B51" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="C51" s="2"/>
+      <c r="C51" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="7"/>
@@ -1777,7 +1854,9 @@
       <c r="B52" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="C52" s="2"/>
+      <c r="C52" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="7"/>
@@ -2059,10 +2138,10 @@
         <v>136</v>
       </c>
       <c r="B75" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C75" s="18" t="s">
         <v>152</v>
-      </c>
-      <c r="C75" s="18" t="s">
-        <v>153</v>
       </c>
       <c r="D75" s="19"/>
       <c r="E75" s="20"/>
@@ -2073,10 +2152,10 @@
         <v>137</v>
       </c>
       <c r="B76" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C76" s="18" t="s">
         <v>154</v>
-      </c>
-      <c r="C76" s="18" t="s">
-        <v>155</v>
       </c>
       <c r="D76" s="19"/>
       <c r="E76" s="20"/>
@@ -2087,17 +2166,43 @@
         <v>146</v>
       </c>
       <c r="B77" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C77" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D77" s="19"/>
       <c r="E77" s="20"/>
       <c r="F77" s="14"/>
     </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B78" s="10"/>
+      <c r="C78" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D78" s="19"/>
+      <c r="E78" s="20"/>
+      <c r="F78" s="14"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B79" s="10"/>
+      <c r="C79" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D79" s="19"/>
+      <c r="E79" s="20"/>
+      <c r="F79" s="14"/>
+    </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="18">
+    <mergeCell ref="C78:E78"/>
+    <mergeCell ref="C79:E79"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C75:E75"/>
     <mergeCell ref="C76:E76"/>

</xml_diff>

<commit_message>
Memory_Expansion_Daughter_Board: Updated checklist for all schematic and pcb layout itens, question marks were placed when there is doubt #6
</commit_message>
<xml_diff>
--- a/Memory_Expansion_Daughter_Board/PCB Design Checklist.xlsx
+++ b/Memory_Expansion_Daughter_Board/PCB Design Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanaz\OneDrive\Área de Trabalho\SpaceLab\FloripaSat-2\Hardware Development\daughter_boards_obdh2\Memory_Expansion_Daughter_Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4260F96-D298-4F71-9F4B-8799E7A9D1A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B256F4-B66D-4B60-95A6-348A9EA4A9A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5735AEBB-7E66-4CF4-B607-EA3656031333}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="175">
   <si>
     <t>1.</t>
   </si>
@@ -524,9 +524,6 @@
     <t>Only 2 layers.</t>
   </si>
   <si>
-    <t>Power width of 0.508mm and all other tracks with 0.254mm.</t>
-  </si>
-  <si>
     <t>No polarity components on project.</t>
   </si>
   <si>
@@ -539,13 +536,28 @@
     <t>OBDH 2.0 responsability.</t>
   </si>
   <si>
-    <t>Initial placement</t>
-  </si>
-  <si>
     <t>4.4</t>
   </si>
   <si>
     <t>4.5</t>
+  </si>
+  <si>
+    <t>Still needs final revision, some may not be acording to standard</t>
+  </si>
+  <si>
+    <t>Power width of 0.508mm and all other tracks with 0.254mm?</t>
+  </si>
+  <si>
+    <t>Not a high speed design</t>
+  </si>
+  <si>
+    <t>Simple design that doesn't require it</t>
+  </si>
+  <si>
+    <t>Initial placement but is not showing hole in drill drawing layer</t>
+  </si>
+  <si>
+    <t>too large table and it is not know how to resize it</t>
   </si>
 </sst>
 </file>
@@ -752,9 +764,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -762,6 +771,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1108,8 +1120,8 @@
   </sheetPr>
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,18 +1129,18 @@
     <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
     </row>
     <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
@@ -1165,7 +1177,7 @@
       </c>
       <c r="E4" s="9">
         <f ca="1">NOW()</f>
-        <v>43886.891437615741</v>
+        <v>43887.794990972223</v>
       </c>
       <c r="F4" s="7"/>
     </row>
@@ -1356,7 +1368,7 @@
         <v>134</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1504,7 +1516,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1528,13 +1540,13 @@
       <c r="B29" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C29" s="2"/>
+      <c r="C29" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D29" s="2"/>
-      <c r="E29" s="2" t="s">
-        <v>134</v>
-      </c>
+      <c r="E29" s="2"/>
       <c r="F29" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1547,7 +1559,9 @@
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="7"/>
+      <c r="F30" s="7" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
@@ -1562,7 +1576,7 @@
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1575,7 +1589,9 @@
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
-      <c r="F32" s="7"/>
+      <c r="F32" s="7" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
@@ -1584,13 +1600,11 @@
       <c r="B33" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>134</v>
-      </c>
+      <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="7" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1693,7 +1707,9 @@
       <c r="E40" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="F40" s="7"/>
+      <c r="F40" s="7" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
@@ -1707,7 +1723,9 @@
       <c r="E41" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="F41" s="7"/>
+      <c r="F41" s="7" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
@@ -1716,12 +1734,12 @@
       <c r="B42" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>134</v>
-      </c>
+      <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
-      <c r="F42" s="7"/>
+      <c r="F42" s="7" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
@@ -1733,7 +1751,9 @@
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
-      <c r="F43" s="7"/>
+      <c r="F43" s="7" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
@@ -1759,7 +1779,9 @@
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
-      <c r="F45" s="7"/>
+      <c r="F45" s="7" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
@@ -1788,7 +1810,7 @@
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="7" t="s">
-        <v>148</v>
+        <v>174</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1802,7 +1824,7 @@
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="7" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1883,7 +1905,9 @@
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
-      <c r="F54" s="7"/>
+      <c r="F54" s="7" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
@@ -1895,7 +1919,9 @@
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
-      <c r="F55" s="7"/>
+      <c r="F55" s="7" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
@@ -1907,7 +1933,9 @@
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
-      <c r="F56" s="7"/>
+      <c r="F56" s="7" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
@@ -1919,7 +1947,9 @@
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
-      <c r="F57" s="7"/>
+      <c r="F57" s="7" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
@@ -1928,7 +1958,9 @@
       <c r="B58" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="C58" s="2"/>
+      <c r="C58" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
       <c r="F58" s="7"/>
@@ -1943,7 +1975,9 @@
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
-      <c r="F59" s="7"/>
+      <c r="F59" s="7" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
@@ -1954,8 +1988,12 @@
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="7"/>
+      <c r="E60" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
@@ -1967,7 +2005,9 @@
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
-      <c r="F61" s="7"/>
+      <c r="F61" s="7" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
@@ -2140,11 +2180,11 @@
       <c r="B75" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="C75" s="18" t="s">
+      <c r="C75" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="D75" s="19"/>
-      <c r="E75" s="20"/>
+      <c r="D75" s="18"/>
+      <c r="E75" s="19"/>
       <c r="F75" s="14"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -2154,11 +2194,11 @@
       <c r="B76" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="C76" s="18" t="s">
+      <c r="C76" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="D76" s="19"/>
-      <c r="E76" s="20"/>
+      <c r="D76" s="18"/>
+      <c r="E76" s="19"/>
       <c r="F76" s="14"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -2168,39 +2208,41 @@
       <c r="B77" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="C77" s="18" t="s">
+      <c r="C77" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="D77" s="19"/>
-      <c r="E77" s="20"/>
+      <c r="D77" s="18"/>
+      <c r="E77" s="19"/>
       <c r="F77" s="14"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B78" s="10"/>
-      <c r="C78" s="18" t="s">
+      <c r="C78" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="D78" s="19"/>
-      <c r="E78" s="20"/>
+      <c r="D78" s="18"/>
+      <c r="E78" s="19"/>
       <c r="F78" s="14"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B79" s="10"/>
-      <c r="C79" s="18" t="s">
+      <c r="C79" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="D79" s="19"/>
-      <c r="E79" s="20"/>
+      <c r="D79" s="18"/>
+      <c r="E79" s="19"/>
       <c r="F79" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C74:E74"/>
     <mergeCell ref="C78:E78"/>
     <mergeCell ref="C79:E79"/>
     <mergeCell ref="A1:F1"/>
@@ -2217,8 +2259,6 @@
     <mergeCell ref="B24:F24"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="B5:F5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C74:E74"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>